<commit_message>
Create ui for flight-search
</commit_message>
<xml_diff>
--- a/documents/Paper Work/01-Sprint_Backlog_A080_Airline_Ticket_Reservation_System_v1.0.xlsx
+++ b/documents/Paper Work/01-Sprint_Backlog_A080_Airline_Ticket_Reservation_System_v1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="8235" activeTab="2"/>
+    <workbookView windowWidth="15360" windowHeight="8235" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Page" sheetId="8" r:id="rId1"/>
@@ -443,10 +443,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="39">
     <font>
@@ -571,14 +571,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -594,14 +586,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -609,8 +593,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -625,15 +624,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -644,6 +637,13 @@
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -662,8 +662,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -677,46 +714,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -797,7 +797,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -815,19 +815,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -839,25 +839,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -875,7 +863,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -887,19 +881,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -911,49 +947,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1168,7 +1168,46 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1207,214 +1246,175 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="21" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="24" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="39" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="23" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="19" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="22" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="29" borderId="22" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="33" fillId="25" borderId="21" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="21" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="20" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="20" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="17" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="15" borderId="22" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="24" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="18" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="18" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="17" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="21" applyFont="true" applyAlignment="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="21" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment vertical="center" wrapText="true"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment vertical="center" wrapText="true"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="21" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
@@ -1433,7 +1433,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="21" applyFont="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true">
@@ -1457,179 +1457,179 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="21" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyAlignment="true" applyProtection="true">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFill="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFill="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="1" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="2" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="11" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="11" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="1" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="2" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="1" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="11" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="2" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="11" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="9" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="49" fontId="16" fillId="9" borderId="2" xfId="2" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" wrapText="true"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="15" fontId="1" fillId="8" borderId="2" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="15" fontId="1" fillId="8" borderId="2" xfId="2" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="center" wrapText="true"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="58" fontId="10" fillId="6" borderId="0" xfId="1" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="58" fontId="10" fillId="6" borderId="0" xfId="2" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="1" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="12" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="2" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyAlignment="true" applyProtection="true">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyAlignment="true" applyProtection="true">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="1" applyFont="true" applyFill="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="1" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="2" applyFont="true" applyFill="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="2" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="1" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="2" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="15" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
       <protection locked="false"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="15" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="15" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="1" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="1" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="2" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="2" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyProtection="true"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyProtection="true"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="13" xfId="1" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="1" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="13" xfId="2" applyFont="true" applyFill="true" applyBorder="true" applyProtection="true"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="2" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 2 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="60% - Accent6" xfId="3" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
     <cellStyle name="60% - Accent5" xfId="5" builtinId="48"/>
@@ -4275,9 +4275,9 @@
   <dimension ref="A1:AA123"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34:D37"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.22" defaultRowHeight="16.5"/>
@@ -8986,9 +8986,6 @@
     <mergeCell ref="D69:D72"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1">
-      <formula1>"Functional, External Interface, User Interface,System Interface, Non functional"</formula1>
-    </dataValidation>
     <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:K27">
       <formula1>0</formula1>
       <formula2>24</formula2>
@@ -8996,6 +8993,9 @@
     <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F27">
       <formula1>0</formula1>
       <formula2>40</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1">
+      <formula1>"Functional, External Interface, User Interface,System Interface, Non functional"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:H1">
       <formula1>"Simple,Average,Complex"</formula1>
@@ -12686,9 +12686,6 @@
     <mergeCell ref="C1:I1"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1">
-      <formula1>"Functional, External Interface, User Interface,System Interface, Non functional"</formula1>
-    </dataValidation>
     <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:K27">
       <formula1>0</formula1>
       <formula2>24</formula2>
@@ -12696,6 +12693,9 @@
     <dataValidation type="decimal" operator="between" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F27">
       <formula1>0</formula1>
       <formula2>40</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1">
+      <formula1>"Functional, External Interface, User Interface,System Interface, Non functional"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:H1">
       <formula1>"Simple,Average,Complex"</formula1>

</xml_diff>